<commit_message>
Finished 8.) RM Breakdown for FG and Sales and 9.) RM Breakdown per JO Report For checking
</commit_message>
<xml_diff>
--- a/Docs/9.) RM Breakdown per JO Report/RMBreakdown_JONo_PONo.xlsx
+++ b/Docs/9.) RM Breakdown per JO Report/RMBreakdown_JONo_PONo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mon\Desktop\LSPI ERP Report Project\GitHub Repo\ERPREPORTS\Docs\9.) RM Breakdown per JO Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C# Projects\ERPREPORTS\Docs\9.) RM Breakdown per JO Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68567CA4-5493-485E-A41B-FF1E0826BBA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADC8467-8DC5-41D6-8822-A4E79F6F8883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB645063-45E2-42D4-864B-13CD0856CC32}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="135">
   <si>
     <t>RM Breakdown</t>
   </si>
@@ -565,7 +565,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -574,24 +584,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,6 +608,219 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2419350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DD623B-A263-4E3C-9C90-E7FF8B42E82C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4352925" y="866775"/>
+          <a:ext cx="6772275" cy="2733675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Speech Bubble: Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56DBA565-AAB5-42E7-89A3-8B57B2125CF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11591925" y="742950"/>
+          <a:ext cx="1828800" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -70833"/>
+            <a:gd name="adj2" fmla="val 51974"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1600"/>
+            <a:t>WHERE Level ==</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1600" baseline="0"/>
+            <a:t> 0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-PH" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Speech Bubble: Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9D24417-0F3B-4684-9F89-1BF343F51E38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12077700" y="3086100"/>
+          <a:ext cx="1828800" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -45312"/>
+            <a:gd name="adj2" fmla="val 104915"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1600"/>
+            <a:t>WHERE Level &gt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1600" baseline="0"/>
+            <a:t> 0</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-PH" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -910,7 +1123,7 @@
   <dimension ref="A1:AJ146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +1170,7 @@
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>126</v>
       </c>
     </row>
@@ -965,31 +1178,31 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="13" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1193,94 +1406,94 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="16" t="s">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="16"/>
-      <c r="AB21" s="16"/>
-      <c r="AC21" s="16"/>
-      <c r="AD21" s="16"/>
-      <c r="AE21" s="16"/>
-      <c r="AF21" s="16"/>
-      <c r="AG21" s="16"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="19"/>
+      <c r="AE21" s="19"/>
+      <c r="AF21" s="19"/>
+      <c r="AG21" s="19"/>
     </row>
     <row r="22" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="13" t="s">
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="12" t="s">
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="13" t="s">
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
-      <c r="AD22" s="13"/>
-      <c r="AE22" s="13"/>
-      <c r="AF22" s="13"/>
-      <c r="AG22" s="13"/>
-      <c r="AH22" s="11" t="s">
+      <c r="AA22" s="17"/>
+      <c r="AB22" s="17"/>
+      <c r="AC22" s="17"/>
+      <c r="AD22" s="17"/>
+      <c r="AE22" s="17"/>
+      <c r="AF22" s="17"/>
+      <c r="AG22" s="17"/>
+      <c r="AH22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="AI22" s="11"/>
-      <c r="AJ22" s="11"/>
+      <c r="AI22" s="14"/>
+      <c r="AJ22" s="14"/>
     </row>
     <row r="23" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1392,113 +1605,113 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:36" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:36" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="L24" s="14" t="s">
+      <c r="L24" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="M24" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="N24" s="14" t="s">
+      <c r="N24" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="O24" s="14" t="s">
+      <c r="O24" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="P24" s="14" t="s">
+      <c r="P24" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="Q24" s="14" t="s">
+      <c r="Q24" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="R24" s="14" t="s">
+      <c r="R24" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="S24" s="14" t="s">
+      <c r="S24" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="T24" s="14" t="s">
+      <c r="T24" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="U24" s="14" t="s">
+      <c r="U24" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="V24" s="14" t="s">
+      <c r="V24" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="W24" s="14" t="s">
+      <c r="W24" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="X24" s="14" t="s">
+      <c r="X24" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="Y24" s="14" t="s">
+      <c r="Y24" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="Z24" s="14" t="s">
+      <c r="Z24" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="AA24" s="14" t="s">
+      <c r="AA24" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="AB24" s="14" t="s">
+      <c r="AB24" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="AC24" s="14" t="s">
+      <c r="AC24" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="AD24" s="14" t="s">
+      <c r="AD24" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="AE24" s="14" t="s">
+      <c r="AE24" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AF24" s="14" t="s">
+      <c r="AF24" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="AG24" s="14" t="s">
+      <c r="AG24" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="AH24" s="14" t="s">
+      <c r="AH24" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="AI24" s="14" t="s">
+      <c r="AI24" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="AJ24" s="14" t="s">
+      <c r="AJ24" s="11" t="s">
         <v>125</v>
       </c>
     </row>
@@ -9447,5 +9660,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>